<commit_message>
New documentation and working with imaging bundles
</commit_message>
<xml_diff>
--- a/Bundles_jul31.xlsx
+++ b/Bundles_jul31.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="36540" yWindow="-440" windowWidth="38400" windowHeight="24000" tabRatio="944" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="944" firstSheet="11" activeTab="32"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2039" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="215">
   <si>
     <t>More</t>
   </si>
@@ -697,6 +697,12 @@
   </si>
   <si>
     <t>This shipment came in thin</t>
+  </si>
+  <si>
+    <t>upside down</t>
+  </si>
+  <si>
+    <t>changed</t>
   </si>
 </sst>
 </file>
@@ -1927,7 +1933,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2013,11 +2018,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2084420504"/>
-        <c:axId val="2083668888"/>
+        <c:axId val="2120740408"/>
+        <c:axId val="2120747560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2084420504"/>
+        <c:axId val="2120740408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2044,13 +2049,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083668888"/>
+        <c:crossAx val="2120747560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2058,7 +2062,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2083668888"/>
+        <c:axId val="2120747560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2080,14 +2084,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2084420504"/>
+        <c:crossAx val="2120740408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2139,7 +2142,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2285,11 +2287,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2086898328"/>
-        <c:axId val="2086892632"/>
+        <c:axId val="2120607816"/>
+        <c:axId val="2120602120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2086898328"/>
+        <c:axId val="2120607816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2316,13 +2318,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086892632"/>
+        <c:crossAx val="2120602120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2330,7 +2331,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2086892632"/>
+        <c:axId val="2120602120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2352,14 +2353,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086898328"/>
+        <c:crossAx val="2120607816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2411,7 +2411,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2557,11 +2556,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2086596376"/>
-        <c:axId val="2086602056"/>
+        <c:axId val="2120561576"/>
+        <c:axId val="2120555880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2086596376"/>
+        <c:axId val="2120561576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2588,13 +2587,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086602056"/>
+        <c:crossAx val="2120555880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2602,7 +2600,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2086602056"/>
+        <c:axId val="2120555880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2624,14 +2622,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086596376"/>
+        <c:crossAx val="2120561576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2829,11 +2826,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2019693912"/>
-        <c:axId val="2019688472"/>
+        <c:axId val="2120506744"/>
+        <c:axId val="2120501288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2019693912"/>
+        <c:axId val="2120506744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2861,7 +2858,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2019688472"/>
+        <c:crossAx val="2120501288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2869,7 +2866,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2019688472"/>
+        <c:axId val="2120501288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2898,7 +2895,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2019693912"/>
+        <c:crossAx val="2120506744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2950,7 +2947,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3096,11 +3092,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2019647976"/>
-        <c:axId val="2019642280"/>
+        <c:axId val="2120460920"/>
+        <c:axId val="2120455224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2019647976"/>
+        <c:axId val="2120460920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3127,13 +3123,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2019642280"/>
+        <c:crossAx val="2120455224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3141,7 +3136,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2019642280"/>
+        <c:axId val="2120455224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3163,14 +3158,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2019647976"/>
+        <c:crossAx val="2120460920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3222,7 +3216,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3338,11 +3331,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2086844952"/>
-        <c:axId val="2086839192"/>
+        <c:axId val="2120403192"/>
+        <c:axId val="2120397432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2086844952"/>
+        <c:axId val="2120403192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3369,13 +3362,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086839192"/>
+        <c:crossAx val="2120397432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3383,7 +3375,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2086839192"/>
+        <c:axId val="2120397432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3405,14 +3397,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086844952"/>
+        <c:crossAx val="2120403192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3464,7 +3455,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3580,11 +3570,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2086798616"/>
-        <c:axId val="2086792856"/>
+        <c:axId val="2120356808"/>
+        <c:axId val="2120351048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2086798616"/>
+        <c:axId val="2120356808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3611,13 +3601,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086792856"/>
+        <c:crossAx val="2120351048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3625,7 +3614,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2086792856"/>
+        <c:axId val="2120351048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3647,14 +3636,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086798616"/>
+        <c:crossAx val="2120356808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3706,7 +3694,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3876,11 +3863,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2086738728"/>
-        <c:axId val="2086733032"/>
+        <c:axId val="2120296968"/>
+        <c:axId val="2120291272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2086738728"/>
+        <c:axId val="2120296968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3907,13 +3894,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086733032"/>
+        <c:crossAx val="2120291272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3921,7 +3907,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2086733032"/>
+        <c:axId val="2120291272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3943,14 +3929,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086738728"/>
+        <c:crossAx val="2120296968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4002,7 +3987,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4130,11 +4114,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2086682776"/>
-        <c:axId val="2086677016"/>
+        <c:axId val="2120241320"/>
+        <c:axId val="2120235560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2086682776"/>
+        <c:axId val="2120241320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4161,13 +4145,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086677016"/>
+        <c:crossAx val="2120235560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4175,7 +4158,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2086677016"/>
+        <c:axId val="2120235560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4197,14 +4180,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086682776"/>
+        <c:crossAx val="2120241320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4256,7 +4238,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4420,11 +4401,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2114225224"/>
-        <c:axId val="2114230904"/>
+        <c:axId val="2132250760"/>
+        <c:axId val="2132256440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2114225224"/>
+        <c:axId val="2132250760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4451,13 +4432,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114230904"/>
+        <c:crossAx val="2132256440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4465,7 +4445,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2114230904"/>
+        <c:axId val="2132256440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4487,14 +4467,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114225224"/>
+        <c:crossAx val="2132250760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4546,7 +4525,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4710,11 +4688,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2114273112"/>
-        <c:axId val="2114278792"/>
+        <c:axId val="2132298680"/>
+        <c:axId val="2132304360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2114273112"/>
+        <c:axId val="2132298680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4741,13 +4719,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114278792"/>
+        <c:crossAx val="2132304360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4755,7 +4732,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2114278792"/>
+        <c:axId val="2132304360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4777,14 +4754,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114273112"/>
+        <c:crossAx val="2132298680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4836,7 +4812,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4922,11 +4897,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2087226872"/>
-        <c:axId val="2087232328"/>
+        <c:axId val="2120829832"/>
+        <c:axId val="2120835288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2087226872"/>
+        <c:axId val="2120829832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4948,13 +4923,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087232328"/>
+        <c:crossAx val="2120835288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4962,7 +4936,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2087232328"/>
+        <c:axId val="2120835288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4984,14 +4958,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087226872"/>
+        <c:crossAx val="2120829832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5043,7 +5016,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5153,11 +5125,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2087315464"/>
-        <c:axId val="2087321208"/>
+        <c:axId val="2120918168"/>
+        <c:axId val="2120923912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2087315464"/>
+        <c:axId val="2120918168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5184,13 +5156,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087321208"/>
+        <c:crossAx val="2120923912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5198,7 +5169,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2087321208"/>
+        <c:axId val="2120923912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5220,14 +5191,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087315464"/>
+        <c:crossAx val="2120918168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5274,7 +5244,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5384,11 +5353,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2087379752"/>
-        <c:axId val="2087385496"/>
+        <c:axId val="2120982488"/>
+        <c:axId val="2120988232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2087379752"/>
+        <c:axId val="2120982488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5415,13 +5384,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087385496"/>
+        <c:crossAx val="2120988232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5429,7 +5397,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2087385496"/>
+        <c:axId val="2120988232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5451,14 +5419,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087379752"/>
+        <c:crossAx val="2120982488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5510,7 +5477,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5620,11 +5586,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2087437096"/>
-        <c:axId val="2087442840"/>
+        <c:axId val="2121039864"/>
+        <c:axId val="2121045608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2087437096"/>
+        <c:axId val="2121039864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5651,13 +5617,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087442840"/>
+        <c:crossAx val="2121045608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5665,7 +5630,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2087442840"/>
+        <c:axId val="2121045608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5687,14 +5652,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087437096"/>
+        <c:crossAx val="2121039864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5746,7 +5710,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5856,11 +5819,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2087483224"/>
-        <c:axId val="2087488968"/>
+        <c:axId val="2121085960"/>
+        <c:axId val="2121091704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2087483224"/>
+        <c:axId val="2121085960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5887,13 +5850,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087488968"/>
+        <c:crossAx val="2121091704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5901,7 +5863,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2087488968"/>
+        <c:axId val="2121091704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5923,14 +5885,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087483224"/>
+        <c:crossAx val="2121085960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5982,7 +5943,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6092,11 +6052,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2087551080"/>
-        <c:axId val="2087556824"/>
+        <c:axId val="2121153944"/>
+        <c:axId val="2121159704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2087551080"/>
+        <c:axId val="2121153944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6123,13 +6083,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087556824"/>
+        <c:crossAx val="2121159704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6137,7 +6096,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2087556824"/>
+        <c:axId val="2121159704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6159,14 +6118,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087551080"/>
+        <c:crossAx val="2121153944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6218,7 +6176,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6334,11 +6291,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2087613848"/>
-        <c:axId val="2087619592"/>
+        <c:axId val="2121216808"/>
+        <c:axId val="2121222568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2087613848"/>
+        <c:axId val="2121216808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6365,13 +6322,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087619592"/>
+        <c:crossAx val="2121222568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6379,7 +6335,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2087619592"/>
+        <c:axId val="2121222568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6401,14 +6357,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087613848"/>
+        <c:crossAx val="2121216808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6460,7 +6415,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6576,11 +6530,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2087662616"/>
-        <c:axId val="2087668376"/>
+        <c:axId val="2120667560"/>
+        <c:axId val="2120661800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2087662616"/>
+        <c:axId val="2120667560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6607,13 +6561,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087668376"/>
+        <c:crossAx val="2120661800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6621,7 +6574,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2087668376"/>
+        <c:axId val="2120661800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6643,14 +6596,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087662616"/>
+        <c:crossAx val="2120667560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -35299,7 +35251,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -36617,7 +36569,7 @@
   <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -36662,7 +36614,9 @@
       <c r="C2" s="185">
         <v>12</v>
       </c>
-      <c r="D2" s="303"/>
+      <c r="D2" s="303" t="s">
+        <v>213</v>
+      </c>
       <c r="E2" s="306">
         <f>AVERAGE(LOOKUP(C2,B!$A$12:$A$165,B!$E$12:$E$165),LOOKUP(C2,B!$A$12:$A$165,B!$F$12:$F$165),LOOKUP(C2,B!$A$12:$A$165,B!$G$12:$G$165),LOOKUP(C2,B!$A$12:$A$165,B!$H$12:$H$165),LOOKUP(C2,B!$A$12:$A$165,B!$I$12:$I$165))</f>
         <v>0.49000000000000005</v>
@@ -40792,7 +40746,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -56720,10 +56674,10 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -56734,7 +56688,7 @@
     <col min="6" max="7" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23">
+    <row r="1" spans="1:8" ht="23">
       <c r="A1" s="304" t="s">
         <v>106</v>
       </c>
@@ -56757,7 +56711,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="87" t="s">
         <v>176</v>
       </c>
@@ -56780,7 +56734,7 @@
         <v>12.91</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" s="87"/>
       <c r="B3" s="185"/>
       <c r="C3" s="185">
@@ -56793,7 +56747,7 @@
       <c r="F3" s="185"/>
       <c r="G3" s="185"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="87"/>
       <c r="B4" s="185"/>
       <c r="C4" s="185">
@@ -56806,7 +56760,7 @@
       <c r="F4" s="185"/>
       <c r="G4" s="185"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="87"/>
       <c r="B5" s="185"/>
       <c r="C5" s="185">
@@ -56819,7 +56773,7 @@
       <c r="F5" s="185"/>
       <c r="G5" s="185"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" s="87"/>
       <c r="B6" s="185" t="s">
         <v>111</v>
@@ -56834,7 +56788,7 @@
       <c r="F6" s="185"/>
       <c r="G6" s="185"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" s="14" t="s">
         <v>177</v>
       </c>
@@ -56851,26 +56805,29 @@
       </c>
       <c r="F7" s="303">
         <f>SUM(E7:E11)+5*1.27</f>
-        <v>12.934999999999999</v>
+        <v>13</v>
       </c>
       <c r="G7" s="303">
         <v>13.09</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="87"/>
       <c r="B8" s="185"/>
       <c r="C8" s="185">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E8" s="306">
         <f>AVERAGE(LOOKUP(C8,G!$A$12:$A$32,G!$E$12:$E$32),LOOKUP(C8,G!$A$12:$A$32,G!$F$12:$F$32),LOOKUP(C8,G!$A$12:$A$32,G!$G$12:$G$32),LOOKUP(C8,G!$A$12:$A$32,G!$H$12:$H$32),LOOKUP(C8,G!$A$12:$A$32,G!$I$12:$I$32),LOOKUP(C8,G!$A$12:$A$32,G!$J$12:$J$32))</f>
-        <v>1.2949999999999999</v>
+        <v>1.36</v>
       </c>
       <c r="F8" s="185"/>
       <c r="G8" s="185"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" s="87"/>
       <c r="B9" s="185"/>
       <c r="C9" s="185">
@@ -56883,7 +56840,7 @@
       <c r="F9" s="185"/>
       <c r="G9" s="185"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" s="87"/>
       <c r="B10" s="185"/>
       <c r="C10" s="185">
@@ -56896,7 +56853,7 @@
       <c r="F10" s="185"/>
       <c r="G10" s="185"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" s="87"/>
       <c r="B11" s="185" t="s">
         <v>111</v>
@@ -56911,7 +56868,7 @@
       <c r="F11" s="185"/>
       <c r="G11" s="185"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" s="14" t="s">
         <v>178</v>
       </c>
@@ -56919,22 +56876,25 @@
         <v>110</v>
       </c>
       <c r="C12" s="303">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D12" s="303"/>
       <c r="E12" s="306">
         <f>AVERAGE(LOOKUP(C12,G!$A$12:$A$32,G!$E$12:$E$32),LOOKUP(C12,G!$A$12:$A$32,G!$F$12:$F$32),LOOKUP(C12,G!$A$12:$A$32,G!$G$12:$G$32),LOOKUP(C12,G!$A$12:$A$32,G!$H$12:$H$32),LOOKUP(C12,G!$A$12:$A$32,G!$I$12:$I$32),LOOKUP(C12,G!$A$12:$A$32,G!$J$12:$J$32))</f>
-        <v>1.36</v>
+        <v>1.2949999999999999</v>
       </c>
       <c r="F12" s="303">
         <f>SUM(E12:E16)+5*1.27</f>
-        <v>12.985000000000001</v>
+        <v>12.966666666666667</v>
       </c>
       <c r="G12" s="303">
         <v>13.06</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="87"/>
       <c r="B13" s="185"/>
       <c r="C13" s="185">
@@ -56947,7 +56907,7 @@
       <c r="F13" s="185"/>
       <c r="G13" s="185"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" s="87"/>
       <c r="B14" s="185"/>
       <c r="C14" s="185">
@@ -56960,35 +56920,41 @@
       <c r="F14" s="185"/>
       <c r="G14" s="185"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" s="87"/>
       <c r="B15" s="185"/>
       <c r="C15" s="185">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>213</v>
       </c>
       <c r="E15" s="306">
         <f>AVERAGE(LOOKUP(C15,G!$A$12:$A$32,G!$E$12:$E$32),LOOKUP(C15,G!$A$12:$A$32,G!$F$12:$F$32),LOOKUP(C15,G!$A$12:$A$32,G!$G$12:$G$32),LOOKUP(C15,G!$A$12:$A$32,G!$H$12:$H$32),LOOKUP(C15,G!$A$12:$A$32,G!$I$12:$I$32),LOOKUP(C15,G!$A$12:$A$32,G!$J$12:$J$32))</f>
-        <v>1.3250000000000002</v>
+        <v>1.3016666666666667</v>
       </c>
       <c r="F15" s="185"/>
       <c r="G15" s="185"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" s="87"/>
       <c r="B16" s="185" t="s">
         <v>111</v>
       </c>
       <c r="C16" s="185">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>213</v>
       </c>
       <c r="E16" s="314">
         <f>AVERAGE(LOOKUP(C16,G!$A$12:$A$32,G!$E$12:$E$32),LOOKUP(C16,G!$A$12:$A$32,G!$F$12:$F$32),LOOKUP(C16,G!$A$12:$A$32,G!$G$12:$G$32),LOOKUP(C16,G!$A$12:$A$32,G!$H$12:$H$32),LOOKUP(C16,G!$A$12:$A$32,G!$I$12:$I$32),LOOKUP(C16,G!$A$12:$A$32,G!$J$12:$J$32))</f>
-        <v>1.2933333333333334</v>
+        <v>1.3633333333333333</v>
       </c>
       <c r="F16" s="185"/>
       <c r="G16" s="185"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" s="14" t="s">
         <v>179</v>
       </c>
@@ -57005,13 +56971,16 @@
       </c>
       <c r="F17" s="303">
         <f>SUM(E17:E21)+5*1.27</f>
-        <v>12.908333333333333</v>
+        <v>12.903333333333332</v>
       </c>
       <c r="G17" s="303">
         <v>13.01</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="87"/>
       <c r="B18" s="185"/>
       <c r="C18" s="185">
@@ -57024,7 +56993,7 @@
       <c r="F18" s="185"/>
       <c r="G18" s="185"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="A19" s="87"/>
       <c r="B19" s="185"/>
       <c r="C19" s="185">
@@ -57037,36 +57006,36 @@
       <c r="F19" s="185"/>
       <c r="G19" s="185"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="A20" s="87"/>
       <c r="B20" s="185"/>
       <c r="C20" s="185">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E20" s="306">
         <f>AVERAGE(LOOKUP(C20,G!$A$12:$A$32,G!$E$12:$E$32),LOOKUP(C20,G!$A$12:$A$32,G!$F$12:$F$32),LOOKUP(C20,G!$A$12:$A$32,G!$G$12:$G$32),LOOKUP(C20,G!$A$12:$A$32,G!$H$12:$H$32),LOOKUP(C20,G!$A$12:$A$32,G!$I$12:$I$32),LOOKUP(C20,G!$A$12:$A$32,G!$J$12:$J$32))</f>
-        <v>1.3016666666666667</v>
+        <v>1.3250000000000002</v>
       </c>
       <c r="F20" s="185"/>
       <c r="G20" s="185"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="A21" s="323"/>
       <c r="B21" s="324" t="s">
         <v>111</v>
       </c>
       <c r="C21" s="324">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D21" s="323"/>
       <c r="E21" s="306">
         <f>AVERAGE(LOOKUP(C21,G!$A$12:$A$32,G!$E$12:$E$32),LOOKUP(C21,G!$A$12:$A$32,G!$F$12:$F$32),LOOKUP(C21,G!$A$12:$A$32,G!$G$12:$G$32),LOOKUP(C21,G!$A$12:$A$32,G!$H$12:$H$32),LOOKUP(C21,G!$A$12:$A$32,G!$I$12:$I$32),LOOKUP(C21,G!$A$12:$A$32,G!$J$12:$J$32))</f>
-        <v>1.3633333333333333</v>
+        <v>1.335</v>
       </c>
       <c r="F21" s="324"/>
       <c r="G21" s="324"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="E22" s="14"/>
     </row>
   </sheetData>
@@ -58219,7 +58188,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -65725,7 +65694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="T42" sqref="T42"/>
     </sheetView>
   </sheetViews>

</xml_diff>